<commit_message>
schema updated by tanvir
</commit_message>
<xml_diff>
--- a/AutomobileSchema.xlsx
+++ b/AutomobileSchema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQL\AutoMobile\Automobile-Assembly-Line\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SQL\Automobile\Automobile-Assembly-Line1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C29F49C-9028-4D38-A26D-5669FF75E4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CCF86E-C7EE-4BFD-B66A-A0F447D8EA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{68985748-78E8-4CB2-B4A8-FEB5F15BAF1B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{68985748-78E8-4CB2-B4A8-FEB5F15BAF1B}"/>
   </bookViews>
   <sheets>
     <sheet name="AutomobileSchema" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Employee_Id</t>
   </si>
@@ -51,68 +42,113 @@
     <t>Customer_Id  (fk)</t>
   </si>
   <si>
-    <t>Customer_Name Varchar2</t>
-  </si>
-  <si>
-    <t>Customer_Id  (PK)  Number</t>
-  </si>
-  <si>
-    <t>City Varchar2</t>
-  </si>
-  <si>
-    <t>Phone_Number Number</t>
-  </si>
-  <si>
-    <t>Gender Varchar2</t>
-  </si>
-  <si>
-    <t>Street_Address Varchar2</t>
-  </si>
-  <si>
-    <t>Car_Type Varchar2</t>
-  </si>
-  <si>
-    <t>Car_Brand Varchar2</t>
-  </si>
-  <si>
     <t>Employee_Id (PK)</t>
   </si>
   <si>
-    <t>Employee_Name</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
     <t>Designation</t>
   </si>
   <si>
-    <t>Commission_Pct</t>
-  </si>
-  <si>
     <t>Department_Id</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Hire_Date</t>
-  </si>
-  <si>
     <t>Product_ID</t>
   </si>
   <si>
     <t>Product_Name</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer_Id  (PK)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer_Name </t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City_Id</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Customer (Dimension)</t>
+  </si>
+  <si>
+    <t>Employees (Dimension)</t>
+  </si>
+  <si>
+    <t>Product (Dimension)</t>
+  </si>
+  <si>
+    <t>Product Category (Dimension0</t>
+  </si>
+  <si>
+    <t>ProductCategoryId</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
+  </si>
+  <si>
+    <t>Department (Dimension)</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Order_Id</t>
+  </si>
+  <si>
+    <t>Order_Date</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Time (Dimension)</t>
+  </si>
+  <si>
+    <t>City (Dimension)</t>
+  </si>
+  <si>
+    <t>City_Name</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,13 +156,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -156,9 +212,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -174,6 +239,538 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>110359</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>98565</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connector: Elbow 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78051D79-DC46-0848-850A-5BD38622CF26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5349766" y="2501462"/>
+          <a:ext cx="1224000" cy="540000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>94594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>21020</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>115614</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Connector: Elbow 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE9C195F-5364-4C89-B0D4-194ED47CBFFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8208579" y="2485697"/>
+          <a:ext cx="1003738" cy="204951"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1418896</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>26276</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>99848</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Connector: Elbow 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBB2F05F-121F-4718-97D7-2AD4F9F84F70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10610193" y="2680138"/>
+          <a:ext cx="1051035" cy="362607"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>21021</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>120869</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>15765</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>99848</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connector: Elbow 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF678436-9EB9-4247-96B7-99572EB410A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10636469" y="4167352"/>
+          <a:ext cx="1014248" cy="530772"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>94594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>404649</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>94594</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDD67551-7098-4A7D-BB64-C4BB94A341B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8208579" y="2485697"/>
+          <a:ext cx="404649" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1056290</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>115615</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10510</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>89339</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Connector: Elbow 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACBCF44B-DC90-4CEB-99EE-BCFB9E543C22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="5323490" y="4162098"/>
+          <a:ext cx="1255986" cy="525517"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1655526</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>121202</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>101959</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="Connector: Elbow 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A792C730-8CB8-4332-A571-11BFF04B00DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8245216" y="2857963"/>
+          <a:ext cx="1714446" cy="1257911"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>472226</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>144887</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>477591</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>150254</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Straight Connector 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3FC2A9F-A758-722F-BDB8-E933EFEAEB28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8725437" y="2699197"/>
+          <a:ext cx="5365" cy="1464972"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1658620</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>132188</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>458953</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>132188</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="82" name="Straight Arrow Connector 81">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB66C544-F489-91E1-14EA-5DD586614973}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8227060" y="4155548"/>
+          <a:ext cx="461493" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1659945</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>160534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>464531</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>164721</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="84" name="Straight Connector 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6813921E-8961-556F-0362-486C0ADC53C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8236861" y="2712246"/>
+          <a:ext cx="464736" cy="4187"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,136 +1070,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7830EB46-BD69-41AB-9BCA-1C4B78BF74C5}">
-  <dimension ref="K2:N28"/>
+  <dimension ref="H13:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F9" zoomScale="180" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="111" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.21875" customWidth="1"/>
+    <col min="12" max="12" width="24.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" customWidth="1"/>
+    <col min="16" max="16" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="M2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="M3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="M4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="M5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="M6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="M7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="M8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="M9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H15" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="K15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="M15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H16" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="K16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="M16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="K18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="K19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="K20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N17" s="1" t="s">
+      <c r="P23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="N20" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="N21" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="N22" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L25" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L27" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="L28" s="1" t="s">
-        <v>23</v>
+    <row r="28" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="M28" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>